<commit_message>
Writing data to excel file at runtime
</commit_message>
<xml_diff>
--- a/Python_Excel/sample.xlsx
+++ b/Python_Excel/sample.xlsx
@@ -1,105 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python-Programs\Python_Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee" sheetId="1" r:id="rId1"/>
-    <sheet name="DEPT" sheetId="2" r:id="rId2"/>
+    <sheet name="Employee" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DEPT" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
-  <si>
-    <t>EMP_ID</t>
-  </si>
-  <si>
-    <t>FIRST_NAME</t>
-  </si>
-  <si>
-    <t>LAST_NAME</t>
-  </si>
-  <si>
-    <t>DEPT</t>
-  </si>
-  <si>
-    <t>SAL</t>
-  </si>
-  <si>
-    <t>ROHIT</t>
-  </si>
-  <si>
-    <t>DESHBHRATAR</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>ANVIKA</t>
-  </si>
-  <si>
-    <t>DETHE</t>
-  </si>
-  <si>
-    <t>R&amp;D</t>
-  </si>
-  <si>
-    <t>RICHA</t>
-  </si>
-  <si>
-    <t>KAMBLE</t>
-  </si>
-  <si>
-    <t>ACCOUNT</t>
-  </si>
-  <si>
-    <t>DEPT_ID</t>
-  </si>
-  <si>
-    <t>DEPT_NAME</t>
-  </si>
-  <si>
-    <t>ASHA</t>
-  </si>
-  <si>
-    <t>WANKAR</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -118,24 +47,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -401,103 +389,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col width="13.140625" customWidth="1" min="2" max="2"/>
+    <col width="14.28515625" customWidth="1" min="3" max="3"/>
+    <col width="10.140625" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>EMP_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>FIRST_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>LAST_NAME</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>DEPT</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ROHIT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DESHBHRATAR</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" t="n">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ASHA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>WANKAR</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>71000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="n">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ANVIKA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DETHE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>R&amp;D</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>77000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" t="n">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RICHA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>KAMBLE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ACCOUNT</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>60000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>105</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Viraj</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wankar</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>90000</v>
       </c>
     </row>
   </sheetData>
@@ -506,56 +555,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>DEPT_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DEPT_NAME</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ACCOUNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R&amp;D</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new excel sheet to workbook
</commit_message>
<xml_diff>
--- a/Python_Excel/sample.xlsx
+++ b/Python_Excel/sample.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Employee" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Department" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Student" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -636,4 +637,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge and unmerge cells using openpyxl
</commit_message>
<xml_diff>
--- a/Python_Excel/sample.xlsx
+++ b/Python_Excel/sample.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Department" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Student" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sort" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Merge" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -47,11 +49,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,11 +404,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.140625" customWidth="1" min="2" max="2"/>
-    <col width="14.28515625" customWidth="1" min="3" max="3"/>
-    <col width="10.140625" customWidth="1" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="14.28515625" customWidth="1" style="2" min="3" max="3"/>
+    <col width="10.140625" customWidth="1" style="2" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -567,9 +570,9 @@
       <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" style="2" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -647,7 +650,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -788,4 +791,130 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.28515625" customWidth="1" style="2" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>40</v>
+      </c>
+      <c r="B3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>93</v>
+      </c>
+      <c r="B4" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B5" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>80</v>
+      </c>
+      <c r="B6" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>21</v>
+      </c>
+      <c r="B7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>63</v>
+      </c>
+      <c r="B8" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>34</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>80</v>
+      </c>
+      <c r="B10" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>20</v>
+      </c>
+      <c r="B11" t="n">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F9:J15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
insert delete rows in excel
</commit_message>
<xml_diff>
--- a/Python_Excel/sample.xlsx
+++ b/Python_Excel/sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,6 +11,7 @@
     <sheet name="Student" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sort" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Merge" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Insert Row" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -29,12 +30,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.5999938962981048"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,11 +56,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,11 +413,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="13.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="14.28515625" customWidth="1" style="2" min="3" max="3"/>
-    <col width="10.140625" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.140625" customWidth="1" style="4" min="2" max="2"/>
+    <col width="14.28515625" customWidth="1" style="4" min="3" max="3"/>
+    <col width="10.140625" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -570,9 +579,9 @@
       <selection activeCell="A1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="16" customWidth="1" style="2" min="2" max="2"/>
+    <col width="16" customWidth="1" style="4" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -805,9 +814,9 @@
       <selection activeCell="H15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="11.28515625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="11.28515625" customWidth="1" style="4" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -896,7 +905,7 @@
   </sheetPr>
   <dimension ref="A3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
@@ -917,4 +926,254 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:T17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
+      <c r="I3" s="2" t="n"/>
+      <c r="J3" s="2" t="n"/>
+      <c r="K3" s="2" t="n"/>
+      <c r="L3" s="2" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="2" t="n"/>
+      <c r="Q3" s="2" t="n"/>
+      <c r="R3" s="2" t="n"/>
+      <c r="S3" s="2" t="n"/>
+      <c r="T3" s="2" t="n"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
+      <c r="K4" s="2" t="n"/>
+      <c r="L4" s="2" t="n"/>
+      <c r="M4" s="2" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="2" t="n"/>
+      <c r="P4" s="2" t="n"/>
+      <c r="Q4" s="2" t="n"/>
+      <c r="R4" s="2" t="n"/>
+      <c r="S4" s="2" t="n"/>
+      <c r="T4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="2" t="n"/>
+      <c r="K5" s="2" t="n"/>
+      <c r="L5" s="2" t="n"/>
+      <c r="M5" s="2" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="2" t="n"/>
+      <c r="P5" s="2" t="n"/>
+      <c r="Q5" s="2" t="n"/>
+      <c r="R5" s="2" t="n"/>
+      <c r="S5" s="2" t="n"/>
+      <c r="T5" s="2" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="2" t="n"/>
+      <c r="K6" s="2" t="n"/>
+      <c r="L6" s="2" t="n"/>
+      <c r="M6" s="2" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="2" t="n"/>
+      <c r="P6" s="2" t="n"/>
+      <c r="Q6" s="2" t="n"/>
+      <c r="R6" s="2" t="n"/>
+      <c r="S6" s="2" t="n"/>
+      <c r="T6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="2" t="n"/>
+      <c r="K7" s="2" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="n"/>
+      <c r="N7" s="2" t="n"/>
+      <c r="O7" s="2" t="n"/>
+      <c r="P7" s="2" t="n"/>
+      <c r="Q7" s="2" t="n"/>
+      <c r="R7" s="2" t="n"/>
+      <c r="S7" s="2" t="n"/>
+      <c r="T7" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
+      <c r="H12" s="2" t="n"/>
+      <c r="I12" s="2" t="n"/>
+      <c r="J12" s="2" t="n"/>
+      <c r="K12" s="2" t="n"/>
+      <c r="L12" s="2" t="n"/>
+      <c r="M12" s="2" t="n"/>
+      <c r="N12" s="2" t="n"/>
+      <c r="O12" s="2" t="n"/>
+      <c r="P12" s="2" t="n"/>
+      <c r="Q12" s="2" t="n"/>
+      <c r="R12" s="2" t="n"/>
+      <c r="S12" s="2" t="n"/>
+      <c r="T12" s="2" t="n"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
+      <c r="K13" s="2" t="n"/>
+      <c r="L13" s="2" t="n"/>
+      <c r="M13" s="2" t="n"/>
+      <c r="N13" s="2" t="n"/>
+      <c r="O13" s="2" t="n"/>
+      <c r="P13" s="2" t="n"/>
+      <c r="Q13" s="2" t="n"/>
+      <c r="R13" s="2" t="n"/>
+      <c r="S13" s="2" t="n"/>
+      <c r="T13" s="2" t="n"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+      <c r="G14" s="2" t="n"/>
+      <c r="H14" s="2" t="n"/>
+      <c r="I14" s="2" t="n"/>
+      <c r="J14" s="2" t="n"/>
+      <c r="K14" s="2" t="n"/>
+      <c r="L14" s="2" t="n"/>
+      <c r="M14" s="2" t="n"/>
+      <c r="N14" s="2" t="n"/>
+      <c r="O14" s="2" t="n"/>
+      <c r="P14" s="2" t="n"/>
+      <c r="Q14" s="2" t="n"/>
+      <c r="R14" s="2" t="n"/>
+      <c r="S14" s="2" t="n"/>
+      <c r="T14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="2" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="2" t="n"/>
+      <c r="M15" s="2" t="n"/>
+      <c r="N15" s="2" t="n"/>
+      <c r="O15" s="2" t="n"/>
+      <c r="P15" s="2" t="n"/>
+      <c r="Q15" s="2" t="n"/>
+      <c r="R15" s="2" t="n"/>
+      <c r="S15" s="2" t="n"/>
+      <c r="T15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="F16" s="2" t="n"/>
+      <c r="G16" s="2" t="n"/>
+      <c r="H16" s="2" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="2" t="n"/>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="2" t="n"/>
+      <c r="M16" s="2" t="n"/>
+      <c r="N16" s="2" t="n"/>
+      <c r="O16" s="2" t="n"/>
+      <c r="P16" s="2" t="n"/>
+      <c r="Q16" s="2" t="n"/>
+      <c r="R16" s="2" t="n"/>
+      <c r="S16" s="2" t="n"/>
+      <c r="T16" s="2" t="n"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="2" t="n"/>
+      <c r="M17" s="2" t="n"/>
+      <c r="N17" s="2" t="n"/>
+      <c r="O17" s="2" t="n"/>
+      <c r="P17" s="2" t="n"/>
+      <c r="Q17" s="2" t="n"/>
+      <c r="R17" s="2" t="n"/>
+      <c r="S17" s="2" t="n"/>
+      <c r="T17" s="2" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add formula to cell
</commit_message>
<xml_diff>
--- a/Python_Excel/sample.xlsx
+++ b/Python_Excel/sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Merge" sheetId="5" r:id="rId5"/>
     <sheet name="Insert Row" sheetId="6" r:id="rId6"/>
     <sheet name="Move Range" sheetId="7" r:id="rId7"/>
+    <sheet name="Formula" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1190,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H4:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4:I7"/>
     </sheetView>
   </sheetViews>
@@ -1231,4 +1232,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>SUM(B5:B11)</f>
+        <v>344</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add logo in excel sheet
</commit_message>
<xml_diff>
--- a/Python_Excel/sample.xlsx
+++ b/Python_Excel/sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,18 @@
     <sheet name="Formula" sheetId="8" r:id="rId8"/>
     <sheet name="Bar Chart" sheetId="9" r:id="rId9"/>
     <sheet name="Line Chart" sheetId="10" r:id="rId10"/>
+    <sheet name="Logo" sheetId="11" r:id="rId11"/>
+    <sheet name="Formatting" sheetId="12" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Formatting!$A$1:$K$11</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>EMP_ID</t>
   </si>
@@ -154,13 +159,77 @@
   </si>
   <si>
     <t>Store</t>
+  </si>
+  <si>
+    <t>Student_Name</t>
+  </si>
+  <si>
+    <t>Marathi</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,10 +261,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,11 +273,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -293,7 +377,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5C33-4DA2-8BE6-CC60790F8F3B}"/>
+              <c16:uniqueId val="{00000000-51DD-4104-BAA1-E2BCA23AF0E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -349,7 +433,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5C33-4DA2-8BE6-CC60790F8F3B}"/>
+              <c16:uniqueId val="{00000001-51DD-4104-BAA1-E2BCA23AF0E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -490,7 +574,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9676-4048-86B6-1D2B59D0D9A3}"/>
+              <c16:uniqueId val="{00000000-2D27-4779-AF76-C83C4101DA9A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -549,7 +633,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9676-4048-86B6-1D2B59D0D9A3}"/>
+              <c16:uniqueId val="{00000001-2D27-4779-AF76-C83C4101DA9A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -601,7 +685,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -671,6 +754,38 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1428750" cy="1428750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="Picture"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -1063,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1158,6 +1273,418 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>55</v>
+      </c>
+      <c r="D2">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
+      </c>
+      <c r="F2">
+        <v>69</v>
+      </c>
+      <c r="G2">
+        <v>62</v>
+      </c>
+      <c r="H2">
+        <v>70</v>
+      </c>
+      <c r="I2" s="4">
+        <f>SUM(C2,D2,E2,F2,G2,H2)</f>
+        <v>377</v>
+      </c>
+      <c r="J2" s="6">
+        <f>((I2/750)*100)</f>
+        <v>50.266666666666673</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>49</v>
+      </c>
+      <c r="H3">
+        <v>52</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I11" si="0">SUM(C3,D3,E3,F3,G3,H3)</f>
+        <v>290</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J11" si="1">((I3/750)*100)</f>
+        <v>38.666666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <v>70</v>
+      </c>
+      <c r="G4">
+        <v>63</v>
+      </c>
+      <c r="H4">
+        <v>72</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>396</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="1"/>
+        <v>52.800000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>41</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>70</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>69</v>
+      </c>
+      <c r="H7">
+        <v>87</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>61.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>70</v>
+      </c>
+      <c r="G8">
+        <v>59</v>
+      </c>
+      <c r="H8">
+        <v>63</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>50.666666666666671</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>49</v>
+      </c>
+      <c r="H9">
+        <v>55</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <v>82</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>71</v>
+      </c>
+      <c r="H10">
+        <v>81</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>491</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="1"/>
+        <v>65.466666666666669</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>56</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>69</v>
+      </c>
+      <c r="G11">
+        <v>65</v>
+      </c>
+      <c r="H11">
+        <v>68</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>48.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1446,60 +1973,60 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>